<commit_message>
Notebook 5 almost finished
</commit_message>
<xml_diff>
--- a/5_correlation_strategy_LM-SEM_local/DataRMSE.xlsx
+++ b/5_correlation_strategy_LM-SEM_local/DataRMSE.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serra\Desktop\CLEMSite Paper\Latest\clemsite-notebooks\5_correlation_strategy_LM-SEM_local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1791F-1C17-4B91-A6AC-264B8F869D56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8911B665-E454-4FA0-AD58-C90046176C48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAA91B73-E517-4F33-87A4-6B3E4E584D5B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration results CLEMSite" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2M_field--X02--Y16_0036</t>
   </si>
@@ -147,6 +146,12 @@
   </si>
   <si>
     <t>43_FAM177B_X02--Y23_0043</t>
+  </si>
+  <si>
+    <t>4N_field--X01--Y16_0013</t>
+  </si>
+  <si>
+    <t>3K_field--X02--Y08_0025</t>
   </si>
 </sst>
 </file>
@@ -225,7 +230,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +258,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
@@ -575,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B5A4D5-54A8-4E6E-9E74-11CC0D2FEF3F}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,15 +1136,15 @@
         <v>498</v>
       </c>
       <c r="E22" s="12">
-        <f xml:space="preserve"> (($C22-512)*0.3)^2</f>
+        <f t="shared" ref="E22:E33" si="3" xml:space="preserve"> (($C22-512)*0.3)^2</f>
         <v>1.44</v>
       </c>
       <c r="F22" s="12">
-        <f xml:space="preserve"> (($D22-512)*0.3)^2</f>
+        <f t="shared" ref="F22:F33" si="4" xml:space="preserve"> (($D22-512)*0.3)^2</f>
         <v>17.64</v>
       </c>
       <c r="G22" s="12">
-        <f>SQRT($F22+$E22)</f>
+        <f t="shared" ref="G22:G33" si="5">SQRT($F22+$E22)</f>
         <v>4.3680659335683112</v>
       </c>
     </row>
@@ -1154,15 +1160,15 @@
         <v>512</v>
       </c>
       <c r="E23" s="12">
-        <f xml:space="preserve"> (($C23-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>2.25</v>
       </c>
       <c r="F23" s="12">
-        <f xml:space="preserve"> (($D23-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G23" s="12">
-        <f>SQRT($F23+$E23)</f>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1178,15 +1184,15 @@
         <v>503</v>
       </c>
       <c r="E24" s="12">
-        <f xml:space="preserve"> (($C24-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>56.25</v>
       </c>
       <c r="F24" s="12">
-        <f xml:space="preserve"> (($D24-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>7.2899999999999983</v>
       </c>
       <c r="G24" s="12">
-        <f>SQRT($F24+$E24)</f>
+        <f t="shared" si="5"/>
         <v>7.9711981533518532</v>
       </c>
     </row>
@@ -1202,15 +1208,15 @@
         <v>499</v>
       </c>
       <c r="E25" s="12">
-        <f xml:space="preserve"> (($C25-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>0.36</v>
       </c>
       <c r="F25" s="12">
-        <f xml:space="preserve"> (($D25-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>15.209999999999999</v>
       </c>
       <c r="G25" s="12">
-        <f>SQRT($F25+$E25)</f>
+        <f t="shared" si="5"/>
         <v>3.9458839313897713</v>
       </c>
     </row>
@@ -1226,15 +1232,15 @@
         <v>519</v>
       </c>
       <c r="E26" s="12">
-        <f xml:space="preserve"> (($C26-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>0.80999999999999983</v>
       </c>
       <c r="F26" s="12">
-        <f xml:space="preserve"> (($D26-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>4.41</v>
       </c>
       <c r="G26" s="12">
-        <f>SQRT($F26+$E26)</f>
+        <f t="shared" si="5"/>
         <v>2.2847319317591723</v>
       </c>
     </row>
@@ -1250,15 +1256,15 @@
         <v>503</v>
       </c>
       <c r="E27" s="12">
-        <f xml:space="preserve"> (($C27-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>1.44</v>
       </c>
       <c r="F27" s="12">
-        <f xml:space="preserve"> (($D27-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>7.2899999999999983</v>
       </c>
       <c r="G27" s="12">
-        <f>SQRT($F27+$E27)</f>
+        <f t="shared" si="5"/>
         <v>2.954657340538831</v>
       </c>
     </row>
@@ -1274,15 +1280,15 @@
         <v>505</v>
       </c>
       <c r="E28" s="12">
-        <f xml:space="preserve"> (($C28-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>26.009999999999998</v>
       </c>
       <c r="F28" s="12">
-        <f xml:space="preserve"> (($D28-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>4.41</v>
       </c>
       <c r="G28" s="12">
-        <f>SQRT($F28+$E28)</f>
+        <f t="shared" si="5"/>
         <v>5.5154328932550705</v>
       </c>
     </row>
@@ -1298,15 +1304,15 @@
         <v>506</v>
       </c>
       <c r="E29" s="12">
-        <f xml:space="preserve"> (($C29-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>5.76</v>
       </c>
       <c r="F29" s="12">
-        <f xml:space="preserve"> (($D29-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>3.2399999999999993</v>
       </c>
       <c r="G29" s="12">
-        <f>SQRT($F29+$E29)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -1322,15 +1328,15 @@
         <v>501</v>
       </c>
       <c r="E30" s="12">
-        <f xml:space="preserve"> (($C30-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>3.2399999999999993</v>
       </c>
       <c r="F30" s="12">
-        <f xml:space="preserve"> (($D30-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>10.889999999999999</v>
       </c>
       <c r="G30" s="12">
-        <f>SQRT($F30+$E30)</f>
+        <f t="shared" si="5"/>
         <v>3.7589892258425004</v>
       </c>
     </row>
@@ -1346,15 +1352,15 @@
         <v>498</v>
       </c>
       <c r="E31" s="12">
-        <f xml:space="preserve"> (($C31-512)*0.3)^2</f>
+        <f t="shared" si="3"/>
         <v>7.2899999999999983</v>
       </c>
       <c r="F31" s="12">
-        <f xml:space="preserve"> (($D31-512)*0.3)^2</f>
+        <f t="shared" si="4"/>
         <v>17.64</v>
       </c>
       <c r="G31" s="12">
-        <f>SQRT($F31+$E31)</f>
+        <f t="shared" si="5"/>
         <v>4.9929950931279716</v>
       </c>
       <c r="I31">
@@ -1367,22 +1373,54 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="A32" s="15">
+        <v>44519</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="14">
+        <v>507</v>
+      </c>
+      <c r="D32" s="14">
+        <v>495</v>
+      </c>
+      <c r="E32" s="14">
+        <f t="shared" si="3"/>
+        <v>2.25</v>
+      </c>
+      <c r="F32" s="14">
+        <f t="shared" si="4"/>
+        <v>26.009999999999998</v>
+      </c>
+      <c r="G32" s="14">
+        <f t="shared" si="5"/>
+        <v>5.3160135440008052</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="B33" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="14">
+        <v>518</v>
+      </c>
+      <c r="D33" s="14">
+        <v>549</v>
+      </c>
+      <c r="E33" s="14">
+        <f t="shared" si="3"/>
+        <v>3.2399999999999993</v>
+      </c>
+      <c r="F33" s="14">
+        <f t="shared" si="4"/>
+        <v>123.21</v>
+      </c>
+      <c r="G33" s="14">
+        <f t="shared" si="5"/>
+        <v>11.244998888394786</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>

</xml_diff>

<commit_message>
Notebook 6 on progress
</commit_message>
<xml_diff>
--- a/5_correlation_strategy_LM-SEM_local/DataRMSE.xlsx
+++ b/5_correlation_strategy_LM-SEM_local/DataRMSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serra\Desktop\CLEMSite Paper\Latest\clemsite-notebooks\5_correlation_strategy_LM-SEM_local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8911B665-E454-4FA0-AD58-C90046176C48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662EAC97-A620-4451-871C-DD81788C5B69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAA91B73-E517-4F33-87A4-6B3E4E584D5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>2M_field--X02--Y16_0036</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>3K_field--X02--Y08_0025</t>
+  </si>
+  <si>
+    <t>5N_field--X02--Y17_0030</t>
+  </si>
+  <si>
+    <t>6H_field--X03--Y05_0037</t>
+  </si>
+  <si>
+    <t>7F_field--X00--Y08_0002</t>
+  </si>
+  <si>
+    <t>6R_field--X01--Y25_0019</t>
   </si>
 </sst>
 </file>
@@ -581,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B5A4D5-54A8-4E6E-9E74-11CC0D2FEF3F}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,15 +1148,15 @@
         <v>498</v>
       </c>
       <c r="E22" s="12">
-        <f t="shared" ref="E22:E33" si="3" xml:space="preserve"> (($C22-512)*0.3)^2</f>
+        <f t="shared" ref="E22:E37" si="3" xml:space="preserve"> (($C22-512)*0.3)^2</f>
         <v>1.44</v>
       </c>
       <c r="F22" s="12">
-        <f t="shared" ref="F22:F33" si="4" xml:space="preserve"> (($D22-512)*0.3)^2</f>
+        <f t="shared" ref="F22:F37" si="4" xml:space="preserve"> (($D22-512)*0.3)^2</f>
         <v>17.64</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" ref="G22:G33" si="5">SQRT($F22+$E22)</f>
+        <f t="shared" ref="G22:G37" si="5">SQRT($F22+$E22)</f>
         <v>4.3680659335683112</v>
       </c>
     </row>
@@ -1398,67 +1410,127 @@
         <v>5.3160135440008052</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="14">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D33" s="14">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E33" s="14">
         <f t="shared" si="3"/>
-        <v>3.2399999999999993</v>
+        <v>1.44</v>
       </c>
       <c r="F33" s="14">
         <f t="shared" si="4"/>
-        <v>123.21</v>
+        <v>116.63999999999997</v>
       </c>
       <c r="G33" s="14">
         <f t="shared" si="5"/>
-        <v>11.244998888394786</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.866462165764899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="14">
+        <v>506</v>
+      </c>
+      <c r="D34" s="14">
+        <v>512</v>
+      </c>
+      <c r="E34" s="14">
+        <f t="shared" si="3"/>
+        <v>3.2399999999999993</v>
+      </c>
+      <c r="F34" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="14">
+        <f t="shared" si="5"/>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="14">
+        <v>514</v>
+      </c>
+      <c r="D35" s="14">
+        <v>526</v>
+      </c>
+      <c r="E35" s="14">
+        <f t="shared" si="3"/>
+        <v>0.36</v>
+      </c>
+      <c r="F35" s="14">
+        <f t="shared" si="4"/>
+        <v>17.64</v>
+      </c>
+      <c r="G35" s="14">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="14">
+        <v>520</v>
+      </c>
+      <c r="D36" s="14">
+        <v>506</v>
+      </c>
+      <c r="E36" s="14">
+        <f t="shared" si="3"/>
+        <v>5.76</v>
+      </c>
+      <c r="F36" s="14">
+        <f t="shared" si="4"/>
+        <v>3.2399999999999993</v>
+      </c>
+      <c r="G36" s="14">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="14">
+        <v>475</v>
+      </c>
+      <c r="D37" s="14">
+        <v>500</v>
+      </c>
+      <c r="E37" s="14">
+        <f t="shared" si="3"/>
+        <v>123.21</v>
+      </c>
+      <c r="F37" s="14">
+        <f t="shared" si="4"/>
+        <v>12.959999999999997</v>
+      </c>
+      <c r="G37" s="14">
+        <f t="shared" si="5"/>
+        <v>11.669190203266034</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
@@ -1467,7 +1539,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="14"/>
@@ -1476,7 +1548,7 @@
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
@@ -1485,7 +1557,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
@@ -1493,6 +1565,14 @@
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
+      <c r="I41">
+        <f>AVERAGE(G32:G41)</f>
+        <v>6.1490511000251713</v>
+      </c>
+      <c r="J41">
+        <f>STDEV(G32:G41)</f>
+        <v>4.1445150118120067</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>